<commit_message>
Implemented the Retry Mechanism and Logs
</commit_message>
<xml_diff>
--- a/testdata/login-data.xlsx
+++ b/testdata/login-data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>emailAddress</t>
   </si>
@@ -33,10 +33,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>narrow@invalid.com</t>
-  </si>
-  <si>
-    <t>NarrowBabe</t>
+    <t>nasrath1298@binafex.com</t>
   </si>
 </sst>
 </file>
@@ -368,12 +365,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -398,7 +395,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -406,6 +403,7 @@
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>